<commit_message>
Info on Grad School
</commit_message>
<xml_diff>
--- a/GradSchool/Opciones.xlsx
+++ b/GradSchool/Opciones.xlsx
@@ -19,6 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$P$7</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>University</t>
   </si>
@@ -383,9 +384,6 @@
     <t>70$</t>
   </si>
   <si>
-    <t>85$</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -417,6 +415,39 @@
   </si>
   <si>
     <t>Required</t>
+  </si>
+  <si>
+    <t>95$</t>
+  </si>
+  <si>
+    <t>General information:
+https://www.vanderbilt.edu/psychological_sciences//graduate/</t>
+  </si>
+  <si>
+    <t>General information:
+http://gsas.nyu.edu/content/nyu-as/gsas/admissions/gsas-application-resource-center/2017-programs--requirements--and-deadlines/psychology.html</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>3 letters of recommendation</t>
+  </si>
+  <si>
+    <t>General information:
+https://apply.grad.ucsd.edu/departments/cognitive-science</t>
+  </si>
+  <si>
+    <t>Minimum of 3 recommendations required.</t>
+  </si>
+  <si>
+    <t>January 1st</t>
+  </si>
+  <si>
+    <t>Institution code 4836</t>
+  </si>
+  <si>
+    <t>125$</t>
   </si>
 </sst>
 </file>
@@ -469,7 +500,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,6 +579,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -921,7 +958,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -953,12 +990,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -971,21 +1002,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -995,24 +1017,15 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1022,9 +1035,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1061,83 +1071,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1436,7 +1494,7 @@
   <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1502,7 @@
     <col min="2" max="2" width="37.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
@@ -1452,191 +1510,191 @@
     <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="12.140625" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" style="69" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="69" customWidth="1"/>
     <col min="16" max="16" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="45" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:30" s="36" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="49" t="s">
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
     </row>
-    <row r="2" spans="1:30" s="45" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="51" t="s">
+    <row r="2" spans="1:30" s="36" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="57" t="s">
+      <c r="M2" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="61" t="s">
+      <c r="N2" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="58" t="s">
+      <c r="O2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="45" customFormat="1" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28">
+    <row r="3" spans="1:30" s="36" customFormat="1" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="60" t="s">
+      <c r="K3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="62" t="s">
+      <c r="L3" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="M3" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="62" t="s">
+      <c r="N3" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="O3" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
-      <c r="AA3" s="43"/>
-      <c r="AB3" s="43"/>
-      <c r="AC3" s="43"/>
-      <c r="AD3" s="44"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34"/>
+      <c r="W3" s="34"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="34"/>
+      <c r="Z3" s="34"/>
+      <c r="AA3" s="34"/>
+      <c r="AB3" s="34"/>
+      <c r="AC3" s="34"/>
+      <c r="AD3" s="35"/>
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71">
+      <c r="A4" s="55">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="60" t="s">
+      <c r="K4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="20" t="s">
+      <c r="N4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="70" t="s">
         <v>28</v>
       </c>
       <c r="P4" s="6" t="s">
@@ -1657,92 +1715,100 @@
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
     </row>
-    <row r="5" spans="1:30" s="1" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" s="37" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="34" t="s">
+      <c r="E5" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="58"/>
+      <c r="M5" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="N5" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="12" t="s">
+      <c r="O5" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="11"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="61"/>
+      <c r="S5" s="61"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="61"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="61"/>
+      <c r="X5" s="61"/>
+      <c r="Y5" s="61"/>
+      <c r="Z5" s="61"/>
+      <c r="AA5" s="61"/>
+      <c r="AB5" s="61"/>
+      <c r="AC5" s="61"/>
+      <c r="AD5" s="62"/>
     </row>
-    <row r="6" spans="1:30" s="1" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" s="1" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18" t="s">
+      <c r="G6" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="27" t="s">
+      <c r="N6" s="26"/>
+      <c r="O6" s="71" t="s">
         <v>45</v>
       </c>
       <c r="P6" s="7" t="s">
@@ -1767,39 +1833,55 @@
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="14" t="s">
+      <c r="C7" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="20"/>
+      <c r="O7" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="15"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:P7">

</xml_diff>